<commit_message>
cambios en los documentos
</commit_message>
<xml_diff>
--- a/LaYumbaVinos/TP Final/Solicitud de Cambio/Solicitud de Cambio - Agregar Clase Conexion.xlsx
+++ b/LaYumbaVinos/TP Final/Solicitud de Cambio/Solicitud de Cambio - Agregar Clase Conexion.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27715"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pgsett/TFI/LaYumbaVinos/TP Final/Solicitud de Cambio/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="5970" windowHeight="6195"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Formato PR-07" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,15 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Formato PR-07'!$B$2:$AX$62</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Formato PR-07'!$2:$3</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -116,19 +129,19 @@
     <t>Solicitud de cambio</t>
   </si>
   <si>
-    <t>Settino German</t>
-  </si>
-  <si>
     <t>Capa DAL</t>
   </si>
   <si>
     <t>Se requiere una clase de conexión para poder cambiar la conexión con la base de datos</t>
   </si>
   <si>
-    <t>Se agrego la clase conexión con 2 metodos getConexionMaster y getConexionFarmacia</t>
+    <t>1 agregar clase en la DAL</t>
   </si>
   <si>
-    <t>1 agregar clase en la DAL</t>
+    <t>Se agrego la clase conexión con 2 metodos getConexionMaster y getConexionLaYumbaVinos</t>
+  </si>
+  <si>
+    <t>Settino Pablo</t>
   </si>
 </sst>
 </file>
@@ -196,10 +209,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -207,7 +220,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -218,171 +231,171 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3134,7 +3147,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-AR" sz="1100"/>
-            <a:t>2015</a:t>
+            <a:t>2016</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3208,7 +3221,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6829425" y="876300"/>
+          <a:off x="8001000" y="860425"/>
           <a:ext cx="327654" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3238,7 +3251,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-AR" sz="1100"/>
-            <a:t>23</a:t>
+            <a:t>20</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3304,7 +3317,7 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1089722" cy="264560"/>
+    <xdr:ext cx="948337" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="6" name="5 CuadroTexto"/>
@@ -3312,8 +3325,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="333375" y="1733550"/>
-          <a:ext cx="1089722" cy="264560"/>
+          <a:off x="381000" y="1708150"/>
+          <a:ext cx="948337" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3342,7 +3355,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-AR" sz="1100"/>
-            <a:t>Settino German</a:t>
+            <a:t>Settino Pablo</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3394,7 +3407,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-AR" sz="1100"/>
-            <a:t>DNI 33633265</a:t>
+            <a:t>DNI 33633264</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3468,7 +3481,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5848350" y="1676400"/>
+          <a:off x="6858000" y="1651000"/>
           <a:ext cx="899605" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3498,7 +3511,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-AR" sz="1100"/>
-            <a:t>1556631551</a:t>
+            <a:t>1558018495</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3599,7 +3612,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="es-AR" sz="1100"/>
-            <a:t>Sistema Farmacia</a:t>
+            <a:t>Sistema La Yumba Vinos</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4057,28 +4070,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja1"/>
+  <sheetPr codeName="Hoja1" enableFormatConditionsCalculation="0"/>
   <dimension ref="B1:BD170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U48" sqref="U48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S46" sqref="S46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="2.28515625" customWidth="1"/>
-    <col min="3" max="28" width="2.42578125" customWidth="1"/>
-    <col min="29" max="29" width="2.5703125" customWidth="1"/>
-    <col min="30" max="39" width="2.42578125" customWidth="1"/>
-    <col min="40" max="49" width="2.28515625" customWidth="1"/>
-    <col min="50" max="50" width="1.5703125" customWidth="1"/>
-    <col min="51" max="51" width="2.28515625" customWidth="1"/>
-    <col min="52" max="79" width="2.42578125" customWidth="1"/>
-    <col min="80" max="84" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="2.33203125" customWidth="1"/>
+    <col min="3" max="39" width="2.5" customWidth="1"/>
+    <col min="40" max="49" width="2.33203125" customWidth="1"/>
+    <col min="50" max="50" width="1.5" customWidth="1"/>
+    <col min="51" max="51" width="2.33203125" customWidth="1"/>
+    <col min="52" max="79" width="2.5" customWidth="1"/>
+    <col min="80" max="84" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:56" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:56" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="P1" s="20" t="s">
         <v>31</v>
       </c>
@@ -4091,8 +4102,8 @@
       <c r="W1" s="20"/>
       <c r="X1" s="20"/>
     </row>
-    <row r="2" spans="2:56" ht="6.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="2:56" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:56" ht="6.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="3" spans="2:56" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="P3" s="2"/>
       <c r="U3" s="29"/>
       <c r="V3" s="30"/>
@@ -4105,7 +4116,7 @@
       <c r="AN3" s="31"/>
       <c r="AO3" s="31"/>
     </row>
-    <row r="4" spans="2:56" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:56" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="34" t="s">
         <v>26</v>
       </c>
@@ -4162,7 +4173,7 @@
       <c r="BC4" s="1"/>
       <c r="BD4" s="1"/>
     </row>
-    <row r="5" spans="2:56" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:56" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="35"/>
       <c r="C5" s="35"/>
       <c r="D5" s="35"/>
@@ -4213,7 +4224,7 @@
       <c r="AW5" s="35"/>
       <c r="AX5" s="35"/>
     </row>
-    <row r="6" spans="2:56" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:56" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C6" s="6" t="s">
         <v>0</v>
       </c>
@@ -4262,7 +4273,7 @@
       <c r="BC6" s="1"/>
       <c r="BD6" s="1"/>
     </row>
-    <row r="7" spans="2:56" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:56" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>
       <c r="D7" s="28"/>
@@ -4312,7 +4323,7 @@
       <c r="AV7" s="1"/>
       <c r="AW7" s="1"/>
     </row>
-    <row r="8" spans="2:56" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:56" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>
       <c r="D8" s="28"/>
@@ -4362,7 +4373,7 @@
       <c r="AV8" s="1"/>
       <c r="AW8" s="1"/>
     </row>
-    <row r="9" spans="2:56" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:56" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="28"/>
       <c r="C9" s="28"/>
       <c r="D9" s="28"/>
@@ -4412,7 +4423,7 @@
       <c r="AV9" s="1"/>
       <c r="AW9" s="1"/>
     </row>
-    <row r="10" spans="2:56" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:56" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="32" t="s">
         <v>17</v>
       </c>
@@ -4455,8 +4466,8 @@
       <c r="AN10" s="11"/>
       <c r="AO10" s="11"/>
     </row>
-    <row r="11" spans="2:56" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="2:56" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:56" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="12" spans="2:56" x14ac:dyDescent="0.15">
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
@@ -4473,15 +4484,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:56" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:56" x14ac:dyDescent="0.15">
       <c r="B13" s="2"/>
       <c r="H13" s="7"/>
       <c r="R13" s="7"/>
       <c r="AA13" s="7"/>
       <c r="AJ13" s="7"/>
     </row>
-    <row r="14" spans="2:56" ht="6.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="2:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:56" ht="6.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="2:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="19" t="s">
         <v>8</v>
       </c>
@@ -4489,7 +4500,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="2:56" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:56" ht="6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="33"/>
       <c r="C16" s="33"/>
       <c r="D16" s="33"/>
@@ -4540,7 +4551,7 @@
       <c r="AW16" s="33"/>
       <c r="AX16" s="33"/>
     </row>
-    <row r="17" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:52" x14ac:dyDescent="0.15">
       <c r="B17" s="15" t="s">
         <v>13</v>
       </c>
@@ -4583,9 +4594,9 @@
       <c r="AM17" s="3"/>
       <c r="AN17" s="3"/>
     </row>
-    <row r="18" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="27"/>
       <c r="D18" s="27"/>
@@ -4636,7 +4647,7 @@
       <c r="AW18" s="27"/>
       <c r="AX18" s="27"/>
     </row>
-    <row r="19" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="27"/>
       <c r="C19" s="27"/>
       <c r="D19" s="27"/>
@@ -4687,7 +4698,7 @@
       <c r="AW19" s="27"/>
       <c r="AX19" s="27"/>
     </row>
-    <row r="20" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="24"/>
       <c r="C20" s="25"/>
       <c r="D20" s="25"/>
@@ -4738,7 +4749,7 @@
       <c r="AW20" s="25"/>
       <c r="AX20" s="26"/>
     </row>
-    <row r="21" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:52" x14ac:dyDescent="0.15">
       <c r="B21" s="6" t="s">
         <v>14</v>
       </c>
@@ -4782,9 +4793,9 @@
       <c r="AN21" s="1"/>
       <c r="AO21" s="1"/>
     </row>
-    <row r="22" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:52" x14ac:dyDescent="0.15">
       <c r="B22" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="27"/>
       <c r="D22" s="27"/>
@@ -4835,7 +4846,7 @@
       <c r="AW22" s="27"/>
       <c r="AX22" s="27"/>
     </row>
-    <row r="23" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:52" x14ac:dyDescent="0.15">
       <c r="B23" s="24"/>
       <c r="C23" s="25"/>
       <c r="D23" s="25"/>
@@ -4886,7 +4897,7 @@
       <c r="AW23" s="25"/>
       <c r="AX23" s="26"/>
     </row>
-    <row r="24" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="24"/>
       <c r="C24" s="25"/>
       <c r="D24" s="25"/>
@@ -4937,7 +4948,7 @@
       <c r="AW24" s="25"/>
       <c r="AX24" s="26"/>
     </row>
-    <row r="25" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="24"/>
       <c r="C25" s="25"/>
       <c r="D25" s="25"/>
@@ -4990,7 +5001,7 @@
       <c r="AY25" s="1"/>
       <c r="AZ25" s="1"/>
     </row>
-    <row r="26" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:52" x14ac:dyDescent="0.15">
       <c r="B26" s="24"/>
       <c r="C26" s="25"/>
       <c r="D26" s="25"/>
@@ -5041,7 +5052,7 @@
       <c r="AW26" s="25"/>
       <c r="AX26" s="26"/>
     </row>
-    <row r="27" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:52" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="24"/>
       <c r="C27" s="25"/>
       <c r="D27" s="25"/>
@@ -5094,7 +5105,7 @@
       <c r="AY27" s="1"/>
       <c r="AZ27" s="1"/>
     </row>
-    <row r="28" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:52" x14ac:dyDescent="0.15">
       <c r="B28" s="27"/>
       <c r="C28" s="27"/>
       <c r="D28" s="27"/>
@@ -5145,7 +5156,7 @@
       <c r="AW28" s="27"/>
       <c r="AX28" s="27"/>
     </row>
-    <row r="29" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:52" x14ac:dyDescent="0.15">
       <c r="B29" s="6" t="s">
         <v>27</v>
       </c>
@@ -5189,7 +5200,7 @@
       <c r="AN29" s="1"/>
       <c r="AO29" s="1"/>
     </row>
-    <row r="30" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:52" x14ac:dyDescent="0.15">
       <c r="B30" s="27" t="s">
         <v>35</v>
       </c>
@@ -5242,7 +5253,7 @@
       <c r="AW30" s="27"/>
       <c r="AX30" s="27"/>
     </row>
-    <row r="31" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="27"/>
       <c r="C31" s="27"/>
       <c r="D31" s="27"/>
@@ -5293,7 +5304,7 @@
       <c r="AW31" s="27"/>
       <c r="AX31" s="27"/>
     </row>
-    <row r="32" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="24"/>
       <c r="C32" s="25"/>
       <c r="D32" s="25"/>
@@ -5344,7 +5355,7 @@
       <c r="AW32" s="25"/>
       <c r="AX32" s="26"/>
     </row>
-    <row r="33" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="24"/>
       <c r="C33" s="25"/>
       <c r="D33" s="25"/>
@@ -5395,7 +5406,7 @@
       <c r="AW33" s="25"/>
       <c r="AX33" s="26"/>
     </row>
-    <row r="34" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="24"/>
       <c r="C34" s="25"/>
       <c r="D34" s="25"/>
@@ -5446,7 +5457,7 @@
       <c r="AW34" s="25"/>
       <c r="AX34" s="26"/>
     </row>
-    <row r="35" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:52" x14ac:dyDescent="0.15">
       <c r="B35" s="6" t="s">
         <v>28</v>
       </c>
@@ -5490,7 +5501,7 @@
       <c r="AN35" s="1"/>
       <c r="AO35" s="1"/>
     </row>
-    <row r="36" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:52" x14ac:dyDescent="0.15">
       <c r="B36" s="22"/>
       <c r="C36" s="21"/>
       <c r="D36" s="21"/>
@@ -5541,7 +5552,7 @@
       <c r="AW36" s="21"/>
       <c r="AX36" s="23"/>
     </row>
-    <row r="37" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:52" x14ac:dyDescent="0.15">
       <c r="B37" s="22"/>
       <c r="C37" s="21"/>
       <c r="D37" s="21"/>
@@ -5594,7 +5605,7 @@
       <c r="AY37" s="1"/>
       <c r="AZ37" s="1"/>
     </row>
-    <row r="38" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="22"/>
       <c r="C38" s="21"/>
       <c r="D38" s="21"/>
@@ -5645,7 +5656,7 @@
       <c r="AW38" s="21"/>
       <c r="AX38" s="23"/>
     </row>
-    <row r="39" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:52" x14ac:dyDescent="0.15">
       <c r="B39" s="24"/>
       <c r="C39" s="25"/>
       <c r="D39" s="25"/>
@@ -5698,7 +5709,7 @@
       <c r="AY39" s="1"/>
       <c r="AZ39" s="1"/>
     </row>
-    <row r="40" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="27"/>
       <c r="C40" s="27"/>
       <c r="D40" s="27"/>
@@ -5749,7 +5760,7 @@
       <c r="AW40" s="27"/>
       <c r="AX40" s="27"/>
     </row>
-    <row r="41" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:52" x14ac:dyDescent="0.15">
       <c r="B41" s="36" t="s">
         <v>15</v>
       </c>
@@ -5802,7 +5813,7 @@
       <c r="AW41" s="37"/>
       <c r="AX41" s="38"/>
     </row>
-    <row r="42" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B42" s="24"/>
       <c r="C42" s="25"/>
       <c r="D42" s="25"/>
@@ -5853,7 +5864,7 @@
       <c r="AW42" s="25"/>
       <c r="AX42" s="26"/>
     </row>
-    <row r="43" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:52" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
       <c r="D43" s="17"/>
@@ -5904,12 +5915,12 @@
       <c r="AW43" s="17"/>
       <c r="AX43" s="17"/>
     </row>
-    <row r="44" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:52" x14ac:dyDescent="0.15">
       <c r="B44" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="2:52" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:52" x14ac:dyDescent="0.15">
       <c r="B45" s="11"/>
       <c r="C45" s="11" t="s">
         <v>0</v>
@@ -5962,12 +5973,12 @@
       <c r="AW45" s="11"/>
       <c r="AX45" s="11"/>
     </row>
-    <row r="46" spans="2:52" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:52" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -6015,7 +6026,7 @@
       <c r="AW46" s="11"/>
       <c r="AX46" s="11"/>
     </row>
-    <row r="47" spans="2:52" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:52" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
       <c r="D47" s="4"/>
@@ -6066,23 +6077,23 @@
       <c r="AW47" s="11"/>
       <c r="AX47" s="11"/>
     </row>
-    <row r="48" spans="2:52" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:52" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B48" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="2:50" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:50" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B49" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="2:50" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:50" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B50" s="2"/>
     </row>
-    <row r="51" spans="2:50" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:50" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B51" s="2"/>
     </row>
-    <row r="52" spans="2:50" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:50" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B52" s="10" t="s">
         <v>16</v>
       </c>
@@ -6127,7 +6138,7 @@
       <c r="AO52" s="1"/>
       <c r="AP52" s="1"/>
     </row>
-    <row r="53" spans="2:50" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:50" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B53" s="44" t="s">
         <v>9</v>
       </c>
@@ -6182,9 +6193,9 @@
       <c r="AW53" s="42"/>
       <c r="AX53" s="43"/>
     </row>
-    <row r="54" spans="2:50" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:50" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B54" s="45" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C54" s="46"/>
       <c r="D54" s="46"/>
@@ -6237,7 +6248,7 @@
       <c r="AW54" s="47"/>
       <c r="AX54" s="48"/>
     </row>
-    <row r="55" spans="2:50" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:50" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B55" s="45">
         <v>2</v>
       </c>
@@ -6290,7 +6301,7 @@
       <c r="AW55" s="47"/>
       <c r="AX55" s="48"/>
     </row>
-    <row r="56" spans="2:50" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:50" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B56" s="45">
         <v>3</v>
       </c>
@@ -6343,7 +6354,7 @@
       <c r="AW56" s="47"/>
       <c r="AX56" s="48"/>
     </row>
-    <row r="57" spans="2:50" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:50" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B57" s="49">
         <v>4</v>
       </c>
@@ -6396,7 +6407,7 @@
       <c r="AW57" s="51"/>
       <c r="AX57" s="52"/>
     </row>
-    <row r="58" spans="2:50" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:50" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B58" s="10" t="s">
         <v>19</v>
       </c>
@@ -6449,7 +6460,7 @@
       <c r="AW58" s="9"/>
       <c r="AX58" s="9"/>
     </row>
-    <row r="59" spans="2:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B59" s="39" t="s">
         <v>30</v>
       </c>
@@ -6502,7 +6513,7 @@
       <c r="AW59" s="40"/>
       <c r="AX59" s="41"/>
     </row>
-    <row r="60" spans="2:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B60" s="39"/>
       <c r="C60" s="40"/>
       <c r="D60" s="40"/>
@@ -6553,7 +6564,7 @@
       <c r="AW60" s="40"/>
       <c r="AX60" s="41"/>
     </row>
-    <row r="61" spans="2:50" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:50" ht="10.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="AD61" s="2"/>
       <c r="AE61" s="6"/>
       <c r="AF61" s="6"/>
@@ -6567,7 +6578,7 @@
       <c r="AN61" s="1"/>
       <c r="AO61" s="1"/>
     </row>
-    <row r="62" spans="2:50" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:50" ht="9.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
@@ -6609,61 +6620,61 @@
       <c r="AO62" s="4"/>
       <c r="AP62" s="4"/>
     </row>
-    <row r="63" spans="2:50" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="2:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="107" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="108" ht="9.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="111" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="112" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="113" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="114" ht="9.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="115" ht="9.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="117" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="122" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="124" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="125" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="126" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="129" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="138" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="140" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="141" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="143" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="144" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="152" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="153" ht="9" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="154" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="156" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="157" ht="5.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="158" ht="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="159" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="161" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="162" ht="9.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="165" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="166" ht="9.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="169" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="170" ht="9.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="2:50" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="64" spans="2:50" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="66" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="67" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="68" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="69" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="70" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="71" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="72" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="73" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="74" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="75" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="76" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="77" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="78" ht="11.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="80" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="84" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="90" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="91" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="92" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="93" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="107" ht="10.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="108" ht="9.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="111" ht="10.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="112" ht="10.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="113" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="114" ht="9.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="115" ht="9.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="117" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="122" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="124" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="125" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="126" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="129" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="138" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="140" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="141" ht="12" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="143" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="144" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="152" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="153" ht="9" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="154" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="156" ht="18.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="157" ht="5.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="158" ht="22.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="159" ht="16.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="161" ht="10.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="162" ht="9.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="165" ht="10.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="166" ht="9.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="169" ht="10.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="170" ht="9.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="41">
     <mergeCell ref="B40:AX40"/>

</xml_diff>